<commit_message>
edits on harplake folder
</commit_message>
<xml_diff>
--- a/HarpLake/ConfigurationInputsHarp.xlsx
+++ b/HarpLake/ConfigurationInputsHarp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IADO\GLEN Fellowship Program\GFP 1\SOS\HarpLake\1991-2001\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\SOS\HarpLake\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D28"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,30 +488,42 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4000</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>4000</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -520,46 +532,46 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>12</v>
+        <v>713800</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>713800</v>
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8320000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2">
-        <v>8320000</v>
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>3.7</v>
+        <v>0.37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -568,50 +580,50 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.37</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>19</v>
@@ -620,147 +632,132 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>19</v>
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3">
-        <v>6.2</v>
+        <v>2</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>0.8</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25">
-        <v>0.8</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B26" s="3">
         <v>78</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Harp lake ProdStartDay and EndDAy
</commit_message>
<xml_diff>
--- a/HarpLake/ConfigurationInputsHarp.xlsx
+++ b/HarpLake/ConfigurationInputsHarp.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\SOS\HarpLake\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="28455" windowHeight="12525"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="28452" windowHeight="12528"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>#General Parameters</t>
   </si>
@@ -127,6 +132,15 @@
   </si>
   <si>
     <t>g/m2/yr</t>
+  </si>
+  <si>
+    <t>ProdStartDay</t>
+  </si>
+  <si>
+    <t>JulianDay</t>
+  </si>
+  <si>
+    <t>ProdEndDay</t>
   </si>
 </sst>
 </file>
@@ -185,7 +199,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -227,7 +241,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,7 +276,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,19 +485,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -494,14 +508,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -513,7 +527,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -525,7 +539,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -537,7 +551,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -549,7 +563,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -561,7 +575,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -573,7 +587,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -581,7 +595,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -593,7 +607,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -601,7 +615,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -613,7 +627,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -625,7 +639,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -637,7 +651,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -649,7 +663,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -661,7 +675,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -673,7 +687,7 @@
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -684,7 +698,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -696,7 +710,7 @@
       </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -704,7 +718,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -716,7 +730,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -727,7 +741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -738,14 +752,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
@@ -754,6 +768,28 @@
       </c>
       <c r="C26" s="3" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="3">
+        <v>90</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="3">
+        <v>330</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -779,7 +815,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>